<commit_message>
create tables for client and commodity alternative names
</commit_message>
<xml_diff>
--- a/data/name/commodity_with_alternative_names.xlsx
+++ b/data/name/commodity_with_alternative_names.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B03479-1DB6-4DF1-9790-636BFC557C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t>Commodity</t>
   </si>
@@ -188,16 +187,19 @@
     <t>железо</t>
   </si>
   <si>
-    <t>npk-удобрения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дизель </t>
+    <t>brent</t>
+  </si>
+  <si>
+    <t>wti</t>
+  </si>
+  <si>
+    <t>urals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,7 +253,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -528,21 +530,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,22 +555,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -576,7 +587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -584,85 +595,85 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
@@ -673,12 +684,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -686,42 +697,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>50</v>
       </c>
@@ -732,69 +743,69 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -803,31 +814,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C44" sqref="A1:C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -835,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -843,17 +854,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -861,67 +872,67 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
@@ -929,12 +940,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -942,42 +953,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
@@ -988,72 +999,72 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
client model, process diff case for fonding name, rating article and etc
</commit_message>
<xml_diff>
--- a/data/name/commodity_with_alternative_names.xlsx
+++ b/data/name/commodity_with_alternative_names.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A71BCE-7047-4AA0-9A54-0B5513D2B09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68F9AE8-7C51-476D-845A-CDE6D8C914B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>Commodity</t>
   </si>
@@ -189,6 +189,42 @@
   </si>
   <si>
     <t>нефть</t>
+  </si>
+  <si>
+    <t>алюминий</t>
+  </si>
+  <si>
+    <t>дизтопливо</t>
+  </si>
+  <si>
+    <t>дизель</t>
+  </si>
+  <si>
+    <t>нефтяной кокс</t>
+  </si>
+  <si>
+    <t>никель</t>
+  </si>
+  <si>
+    <t>кобальт</t>
+  </si>
+  <si>
+    <t>жрс</t>
+  </si>
+  <si>
+    <t>карбамид</t>
+  </si>
+  <si>
+    <t>аммиачная селитра</t>
+  </si>
+  <si>
+    <t>диаммонийфосфат</t>
+  </si>
+  <si>
+    <t>апатитовый концетрат</t>
+  </si>
+  <si>
+    <t>npk-удобрения</t>
   </si>
 </sst>
 </file>
@@ -529,7 +565,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,10 +614,13 @@
     </row>
     <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
@@ -596,7 +635,7 @@
     </row>
     <row r="9" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
@@ -611,12 +650,12 @@
     </row>
     <row r="12" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
@@ -646,12 +685,12 @@
     </row>
     <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -731,7 +770,7 @@
     </row>
     <row r="33" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
@@ -741,12 +780,12 @@
     </row>
     <row r="35" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
@@ -756,7 +795,7 @@
     </row>
     <row r="38" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
@@ -766,7 +805,7 @@
     </row>
     <row r="40" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
@@ -781,7 +820,7 @@
     </row>
     <row r="43" spans="1:1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>